<commit_message>
Se cambia estructura de proyecto, para trabajar por capas.
</commit_message>
<xml_diff>
--- a/PointSaleBD/Documentacion/00 DefinicionTablas.xlsx
+++ b/PointSaleBD/Documentacion/00 DefinicionTablas.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\12 Proyectos Personales\03 Titulacion\PointSale\PointSaleBD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\12 Proyectos Personales\03 Titulacion\PointSale\PointSaleBD\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7188D64-A5AE-4C29-A844-A0CA62C0B5FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C47EB2E-3C46-448C-BEEE-CCDB02A674ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{48E06636-C132-4209-84F9-2371AB238586}"/>
   </bookViews>
   <sheets>
-    <sheet name="USUARIOS" sheetId="6" r:id="rId1"/>
-    <sheet name="PERSONAS" sheetId="4" r:id="rId2"/>
-    <sheet name="MENU" sheetId="1" r:id="rId3"/>
-    <sheet name="PERFILES" sheetId="3" r:id="rId4"/>
-    <sheet name="ROLES" sheetId="5" r:id="rId5"/>
-    <sheet name="PARAMETROS" sheetId="2" r:id="rId6"/>
+    <sheet name="00 ReglasBD" sheetId="7" r:id="rId1"/>
+    <sheet name="USUARIOS" sheetId="6" r:id="rId2"/>
+    <sheet name="PERSONAS" sheetId="4" r:id="rId3"/>
+    <sheet name="MENU" sheetId="1" r:id="rId4"/>
+    <sheet name="PERFILES" sheetId="3" r:id="rId5"/>
+    <sheet name="ROLES" sheetId="5" r:id="rId6"/>
+    <sheet name="PARAMETROS" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="88">
   <si>
     <t>IdMenu</t>
   </si>
@@ -197,6 +198,114 @@
   </si>
   <si>
     <t>VARCHAR(20)</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Identificador</t>
+  </si>
+  <si>
+    <t>Catalogo</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Sistema</t>
+  </si>
+  <si>
+    <t>Trnasaccional</t>
+  </si>
+  <si>
+    <t>Tipo accion</t>
+  </si>
+  <si>
+    <t>Numerador</t>
+  </si>
+  <si>
+    <t>Select</t>
+  </si>
+  <si>
+    <t>Insert</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>Del</t>
+  </si>
+  <si>
+    <t>Sel</t>
+  </si>
+  <si>
+    <t>Ins</t>
+  </si>
+  <si>
+    <t>Upd</t>
+  </si>
+  <si>
+    <t>Ejemplo</t>
+  </si>
+  <si>
+    <t>CTACOS</t>
+  </si>
+  <si>
+    <t>TVENTA</t>
+  </si>
+  <si>
+    <t>SBITACORA</t>
+  </si>
+  <si>
+    <t>Sel_Tacos_01</t>
+  </si>
+  <si>
+    <t>Ins_Tacos_01</t>
+  </si>
+  <si>
+    <t>Upd_Tacos_01</t>
+  </si>
+  <si>
+    <t>Del_Tacos_01</t>
+  </si>
+  <si>
+    <t>Fn</t>
+  </si>
+  <si>
+    <t>FnDiasHabiles</t>
+  </si>
+  <si>
+    <t>Tgr</t>
+  </si>
+  <si>
+    <t>TgrEliminaRegistro</t>
+  </si>
+  <si>
+    <t>Trigggers</t>
+  </si>
+  <si>
+    <t>Funciones</t>
+  </si>
+  <si>
+    <t>Procedimientos Almacenados</t>
+  </si>
+  <si>
+    <t>Tablas</t>
+  </si>
+  <si>
+    <t>Vistas</t>
+  </si>
+  <si>
+    <t>Vta</t>
+  </si>
+  <si>
+    <t>VtaPago</t>
   </si>
 </sst>
 </file>
@@ -273,10 +382,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -288,6 +397,17 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -406,17 +526,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -749,10 +858,217 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C19C553-447B-4A14-91B3-373D7A1D0B05}">
+  <dimension ref="B2:E25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB0DB3F-5180-4EF8-9E13-2A1EB9707AC2}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -1098,20 +1414,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:J1048576">
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D1:J1048576">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
-      <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFBC40A9-B96E-441F-BF7D-134088CDBBB3}">
   <dimension ref="A1:L10"/>
   <sheetViews>
@@ -1355,20 +1669,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:J1048576">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D1:J1048576">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
-      <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{160DA08D-7B97-48FF-A514-C6A8BFA62206}">
   <dimension ref="A1:L13"/>
   <sheetViews>
@@ -1672,20 +1984,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:J1048576">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D1:J1048576">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
-      <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14C6D8C1-ACA2-4A13-AD85-5D96951EC1E0}">
   <dimension ref="A1:L8"/>
   <sheetViews>
@@ -1889,20 +2199,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:J1048576">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D1:J1048576">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
-      <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{204A916E-B42F-47D9-9E88-96E77FB1E3C8}">
   <dimension ref="A1:L7"/>
   <sheetViews>
@@ -2086,20 +2394,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:J1048576">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D1:J1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
-      <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7319551-CB9A-4ADC-8C14-571A1B175CDA}">
   <dimension ref="A1:L10"/>
   <sheetViews>
@@ -2343,13 +2649,11 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:J1048576">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D1:J1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
definicion de estructura de bd
</commit_message>
<xml_diff>
--- a/PointSaleBD/Documentacion/00 DefinicionTablas.xlsx
+++ b/PointSaleBD/Documentacion/00 DefinicionTablas.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\12 Proyectos Personales\03 Titulacion\PointSale\PointSaleBD\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C47EB2E-3C46-448C-BEEE-CCDB02A674ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAFBEB30-ECB4-4E17-B96D-1F7D10F82741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{48E06636-C132-4209-84F9-2371AB238586}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{48E06636-C132-4209-84F9-2371AB238586}"/>
   </bookViews>
   <sheets>
     <sheet name="00 ReglasBD" sheetId="7" r:id="rId1"/>
-    <sheet name="USUARIOS" sheetId="6" r:id="rId2"/>
-    <sheet name="PERSONAS" sheetId="4" r:id="rId3"/>
-    <sheet name="MENU" sheetId="1" r:id="rId4"/>
-    <sheet name="PERFILES" sheetId="3" r:id="rId5"/>
-    <sheet name="ROLES" sheetId="5" r:id="rId6"/>
-    <sheet name="PARAMETROS" sheetId="2" r:id="rId7"/>
+    <sheet name="Hoja2" sheetId="8" r:id="rId2"/>
+    <sheet name="USUARIOS" sheetId="6" r:id="rId3"/>
+    <sheet name="PERSONAS" sheetId="4" r:id="rId4"/>
+    <sheet name="MENU" sheetId="1" r:id="rId5"/>
+    <sheet name="PERFILES" sheetId="3" r:id="rId6"/>
+    <sheet name="ROLES" sheetId="5" r:id="rId7"/>
+    <sheet name="PARAMETROS" sheetId="2" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -861,8 +862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C19C553-447B-4A14-91B3-373D7A1D0B05}">
   <dimension ref="B2:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,6 +1066,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB682CC2-5C8B-4F26-AD34-1FEBDC7ADCD5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB0DB3F-5180-4EF8-9E13-2A1EB9707AC2}">
   <dimension ref="A1:L12"/>
   <sheetViews>
@@ -1425,7 +1440,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFBC40A9-B96E-441F-BF7D-134088CDBBB3}">
   <dimension ref="A1:L10"/>
   <sheetViews>
@@ -1680,7 +1695,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{160DA08D-7B97-48FF-A514-C6A8BFA62206}">
   <dimension ref="A1:L13"/>
   <sheetViews>
@@ -1995,12 +2010,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14C6D8C1-ACA2-4A13-AD85-5D96951EC1E0}">
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2210,7 +2225,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{204A916E-B42F-47D9-9E88-96E77FB1E3C8}">
   <dimension ref="A1:L7"/>
   <sheetViews>
@@ -2405,7 +2420,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7319551-CB9A-4ADC-8C14-571A1B175CDA}">
   <dimension ref="A1:L10"/>
   <sheetViews>

</xml_diff>